<commit_message>
try to cache the weather
</commit_message>
<xml_diff>
--- a/02_config/example_single_market/agents.xlsx
+++ b/02_config/example_single_market/agents.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="319">
   <si>
     <t>general/agent_id</t>
   </si>
@@ -820,57 +820,57 @@
     <t>ems/fcasts/update</t>
   </si>
   <si>
-    <t>BsIKeyrf1lj3rVO</t>
-  </si>
-  <si>
-    <t>8f3vvlIRj9ICt8O</t>
-  </si>
-  <si>
-    <t>T0trImFXXGMgP9I</t>
-  </si>
-  <si>
-    <t>bZHXZoNjVVbyhNo</t>
-  </si>
-  <si>
-    <t>79O1mruFbVgykmF</t>
-  </si>
-  <si>
-    <t>EVzNaAJab8rA3Go</t>
-  </si>
-  <si>
-    <t>QFcbDCphvAGIikn</t>
-  </si>
-  <si>
-    <t>N0HOa2ZKJcz12gC</t>
-  </si>
-  <si>
-    <t>Ts9tuWCg09uwsSa</t>
-  </si>
-  <si>
-    <t>spIQTuoMuglwLsn</t>
-  </si>
-  <si>
-    <t>hh_2959_0.csv</t>
+    <t>7RoMKhKPykXrFxN</t>
+  </si>
+  <si>
+    <t>ryYqphAYH66rqBR</t>
+  </si>
+  <si>
+    <t>9EzYHF2KmClcoSH</t>
+  </si>
+  <si>
+    <t>To06tKG30CoaBBZ</t>
+  </si>
+  <si>
+    <t>ci3ggclTDIuxx0J</t>
+  </si>
+  <si>
+    <t>8HAaGxfdIuOYpoE</t>
+  </si>
+  <si>
+    <t>li0yQQQ2eFSuKVB</t>
+  </si>
+  <si>
+    <t>S3jFOl27BE4LplR</t>
+  </si>
+  <si>
+    <t>YawQtd5fYkC08f3</t>
+  </si>
+  <si>
+    <t>fkJkOc4Pri4u6sg</t>
+  </si>
+  <si>
+    <t>hh_2532_0.csv</t>
+  </si>
+  <si>
+    <t>hh_4402_0.csv</t>
+  </si>
+  <si>
+    <t>hh_4536_0.csv</t>
+  </si>
+  <si>
+    <t>hh_3125_0.csv</t>
+  </si>
+  <si>
+    <t>hh_3564_0.csv</t>
   </si>
   <si>
     <t>hh_5527_0.csv</t>
   </si>
   <si>
-    <t>hh_2896_0.csv</t>
-  </si>
-  <si>
     <t>hh_3863_0.csv</t>
   </si>
   <si>
-    <t>hh_4536_0.csv</t>
-  </si>
-  <si>
-    <t>hh_3564_0.csv</t>
-  </si>
-  <si>
-    <t>hh_3125_0.csv</t>
-  </si>
-  <si>
     <t>perfect</t>
   </si>
   <si>
@@ -886,28 +886,28 @@
     <t>rfr</t>
   </si>
   <si>
-    <t>heat_2959_0.csv</t>
+    <t>heat_gen_4_pu.csv</t>
+  </si>
+  <si>
+    <t>heat_4402_0.csv</t>
+  </si>
+  <si>
+    <t>heat_gen_0_pu.csv</t>
+  </si>
+  <si>
+    <t>heat_2532_0.csv</t>
+  </si>
+  <si>
+    <t>heat_3125_0.csv</t>
+  </si>
+  <si>
+    <t>heat_3564_0.csv</t>
   </si>
   <si>
     <t>heat_5527_0.csv</t>
   </si>
   <si>
-    <t>heat_gen_0_pu.csv</t>
-  </si>
-  <si>
-    <t>heat_3863_0.csv</t>
-  </si>
-  <si>
-    <t>heat_4536_0.csv</t>
-  </si>
-  <si>
-    <t>heat_gen_5_pu.csv</t>
-  </si>
-  <si>
-    <t>heat_3564_0.csv</t>
-  </si>
-  <si>
-    <t>heat_3125_0.csv</t>
+    <t>heat_gen_1_pu.csv</t>
   </si>
   <si>
     <t>naive</t>
@@ -934,19 +934,22 @@
     <t>hp_DAIKIN Europe_ground.json</t>
   </si>
   <si>
+    <t>ev_freetime_3.csv</t>
+  </si>
+  <si>
     <t>ev_fulltime_48.csv</t>
   </si>
   <si>
-    <t>ev_freetime_1.csv</t>
-  </si>
-  <si>
-    <t>ev_fulltime_47.csv</t>
-  </si>
-  <si>
-    <t>ev_freetime_3.csv</t>
-  </si>
-  <si>
-    <t>ev_fulltime_44.csv</t>
+    <t>ev_freetime_2.csv</t>
+  </si>
+  <si>
+    <t>ev_fulltime_42.csv</t>
+  </si>
+  <si>
+    <t>ev_parttime_88.csv</t>
+  </si>
+  <si>
+    <t>ev_fulltime_45.csv</t>
   </si>
   <si>
     <t>min_soc</t>
@@ -2145,10 +2148,10 @@
         <v>268</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2157,7 +2160,7 @@
         <v>2.6</v>
       </c>
       <c r="J2">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2169,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>2959000</v>
+        <v>2532000</v>
       </c>
       <c r="O2" t="s">
         <v>278</v>
@@ -2298,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="BG2">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH2" t="s">
         <v>290</v>
@@ -2424,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="CZ2">
-        <v>5100</v>
+        <v>4100</v>
       </c>
       <c r="DA2" t="s">
         <v>300</v>
@@ -2628,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="FV2">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW2" t="s">
         <v>304</v>
@@ -2691,67 +2694,13 @@
         <v>303</v>
       </c>
       <c r="GQ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR2">
-        <v>2</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>306</v>
-      </c>
-      <c r="GT2">
-        <v>50000</v>
-      </c>
-      <c r="GU2">
-        <v>7200</v>
-      </c>
-      <c r="GV2">
-        <v>7200</v>
-      </c>
-      <c r="GW2">
-        <v>50000</v>
-      </c>
-      <c r="GX2">
-        <v>0.9</v>
-      </c>
-      <c r="GY2">
-        <v>0.8</v>
-      </c>
-      <c r="GZ2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HB2" t="s">
-        <v>308</v>
-      </c>
-      <c r="HC2">
-        <v>50000</v>
-      </c>
-      <c r="HD2">
-        <v>7200</v>
-      </c>
-      <c r="HE2">
-        <v>7200</v>
-      </c>
-      <c r="HF2">
-        <v>50000</v>
-      </c>
-      <c r="HG2">
-        <v>0.9</v>
-      </c>
-      <c r="HH2">
-        <v>0.8</v>
-      </c>
-      <c r="HI2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HJ2" t="b">
         <v>0</v>
       </c>
       <c r="HK2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL2">
         <v>0.05</v>
@@ -2766,36 +2715,18 @@
         <v>8.5</v>
       </c>
       <c r="HP2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR2" t="s">
         <v>303</v>
       </c>
       <c r="HS2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT2">
-        <v>1</v>
-      </c>
-      <c r="HU2">
-        <v>3000</v>
-      </c>
-      <c r="HV2">
-        <v>3000</v>
-      </c>
-      <c r="HW2">
-        <v>0.95</v>
-      </c>
-      <c r="HX2">
-        <v>0.1</v>
-      </c>
-      <c r="HY2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HZ2" t="b">
         <v>0</v>
       </c>
       <c r="IA2" t="s">
@@ -2808,10 +2739,10 @@
         <v>1</v>
       </c>
       <c r="ID2">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE2">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF2">
         <v>0.95</v>
@@ -2823,43 +2754,43 @@
         <v>303</v>
       </c>
       <c r="II2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK2">
         <v>120</v>
       </c>
       <c r="IL2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM2">
         <v>120</v>
       </c>
       <c r="IN2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO2">
         <v>86400</v>
       </c>
       <c r="IP2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ2">
         <v>120</v>
       </c>
       <c r="IR2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS2">
         <v>120</v>
       </c>
       <c r="IT2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU2">
-        <v>43200</v>
+        <v>57600</v>
       </c>
       <c r="IV2">
         <v>1</v>
@@ -2880,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="JB2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC2" t="s">
         <v>298</v>
@@ -2892,7 +2823,7 @@
         <v>298</v>
       </c>
       <c r="JF2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG2">
         <v>86400</v>
@@ -2912,10 +2843,10 @@
         <v>269</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2924,7 +2855,7 @@
         <v>2.6</v>
       </c>
       <c r="J3">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2936,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>5527000</v>
+        <v>4402000</v>
       </c>
       <c r="O3" t="s">
         <v>279</v>
@@ -3065,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="BG3">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH3" t="s">
         <v>291</v>
@@ -3380,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="FV3">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW3" t="s">
         <v>304</v>
@@ -3449,19 +3380,19 @@
         <v>1</v>
       </c>
       <c r="GS3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="GT3">
+        <v>75000</v>
+      </c>
+      <c r="GU3">
+        <v>7200</v>
+      </c>
+      <c r="GV3">
+        <v>11000</v>
+      </c>
+      <c r="GW3">
         <v>100000</v>
-      </c>
-      <c r="GU3">
-        <v>11000</v>
-      </c>
-      <c r="GV3">
-        <v>22000</v>
-      </c>
-      <c r="GW3">
-        <v>200000</v>
       </c>
       <c r="GX3">
         <v>0.9</v>
@@ -3476,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="HK3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL3">
         <v>0.05</v>
@@ -3491,10 +3422,10 @@
         <v>8.5</v>
       </c>
       <c r="HP3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR3" t="s">
         <v>303</v>
@@ -3515,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="ID3">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE3">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF3">
         <v>0.95</v>
@@ -3530,43 +3461,43 @@
         <v>303</v>
       </c>
       <c r="II3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK3">
         <v>120</v>
       </c>
       <c r="IL3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM3">
         <v>120</v>
       </c>
       <c r="IN3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO3">
         <v>86400</v>
       </c>
       <c r="IP3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ3">
         <v>120</v>
       </c>
       <c r="IR3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS3">
         <v>120</v>
       </c>
       <c r="IT3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU3">
-        <v>57600</v>
+        <v>86400</v>
       </c>
       <c r="IV3">
         <v>1</v>
@@ -3587,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="JB3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC3" t="s">
         <v>298</v>
@@ -3599,7 +3530,7 @@
         <v>298</v>
       </c>
       <c r="JF3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG3">
         <v>86400</v>
@@ -3619,10 +3550,10 @@
         <v>270</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -3631,7 +3562,7 @@
         <v>2.6</v>
       </c>
       <c r="J4">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -3643,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>2896000</v>
+        <v>4536000</v>
       </c>
       <c r="O4" t="s">
         <v>280</v>
@@ -3772,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="BG4">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH4" t="s">
         <v>292</v>
@@ -3892,9 +3823,24 @@
         <v>3</v>
       </c>
       <c r="CX4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CY4">
+        <v>1</v>
+      </c>
+      <c r="CZ4">
+        <v>7600</v>
+      </c>
+      <c r="DA4" t="s">
+        <v>300</v>
+      </c>
+      <c r="DB4">
+        <v>0</v>
+      </c>
+      <c r="DC4">
+        <v>40</v>
+      </c>
+      <c r="DD4" t="b">
         <v>0</v>
       </c>
       <c r="DE4" t="s">
@@ -4087,7 +4033,7 @@
         <v>1</v>
       </c>
       <c r="FV4">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW4" t="s">
         <v>304</v>
@@ -4150,40 +4096,13 @@
         <v>303</v>
       </c>
       <c r="GQ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR4">
-        <v>1</v>
-      </c>
-      <c r="GS4" t="s">
-        <v>308</v>
-      </c>
-      <c r="GT4">
-        <v>75000</v>
-      </c>
-      <c r="GU4">
-        <v>7200</v>
-      </c>
-      <c r="GV4">
-        <v>11000</v>
-      </c>
-      <c r="GW4">
-        <v>100000</v>
-      </c>
-      <c r="GX4">
-        <v>0.9</v>
-      </c>
-      <c r="GY4">
-        <v>0.8</v>
-      </c>
-      <c r="GZ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA4" t="b">
         <v>0</v>
       </c>
       <c r="HK4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL4">
         <v>0.05</v>
@@ -4198,18 +4117,36 @@
         <v>8.5</v>
       </c>
       <c r="HP4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR4" t="s">
         <v>303</v>
       </c>
       <c r="HS4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HT4">
+        <v>1</v>
+      </c>
+      <c r="HU4">
+        <v>4500</v>
+      </c>
+      <c r="HV4">
+        <v>4500</v>
+      </c>
+      <c r="HW4">
+        <v>0.95</v>
+      </c>
+      <c r="HX4">
+        <v>0.1</v>
+      </c>
+      <c r="HY4" t="b">
+        <v>0</v>
+      </c>
+      <c r="HZ4" t="b">
         <v>0</v>
       </c>
       <c r="IA4" t="s">
@@ -4222,10 +4159,10 @@
         <v>1</v>
       </c>
       <c r="ID4">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE4">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF4">
         <v>0.95</v>
@@ -4237,40 +4174,40 @@
         <v>303</v>
       </c>
       <c r="II4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK4">
         <v>120</v>
       </c>
       <c r="IL4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM4">
         <v>120</v>
       </c>
       <c r="IN4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO4">
         <v>86400</v>
       </c>
       <c r="IP4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ4">
         <v>120</v>
       </c>
       <c r="IR4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS4">
         <v>120</v>
       </c>
       <c r="IT4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU4">
         <v>57600</v>
@@ -4294,7 +4231,7 @@
         <v>1</v>
       </c>
       <c r="JB4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC4" t="s">
         <v>298</v>
@@ -4306,7 +4243,7 @@
         <v>298</v>
       </c>
       <c r="JF4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG4">
         <v>86400</v>
@@ -4326,10 +4263,10 @@
         <v>271</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -4338,7 +4275,7 @@
         <v>2.6</v>
       </c>
       <c r="J5">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -4350,10 +4287,10 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>3863000</v>
+        <v>2532000</v>
       </c>
       <c r="O5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="P5" t="s">
         <v>285</v>
@@ -4479,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="BG5">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH5" t="s">
         <v>293</v>
@@ -4605,16 +4542,16 @@
         <v>1</v>
       </c>
       <c r="CZ5">
-        <v>5700</v>
+        <v>3800</v>
       </c>
       <c r="DA5" t="s">
         <v>300</v>
       </c>
       <c r="DB5">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="DC5">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="DD5" t="b">
         <v>0</v>
@@ -4809,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="FV5">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW5" t="s">
         <v>304</v>
@@ -4878,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="HK5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL5">
         <v>0.05</v>
@@ -4893,10 +4830,10 @@
         <v>8.5</v>
       </c>
       <c r="HP5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR5" t="s">
         <v>303</v>
@@ -4908,10 +4845,10 @@
         <v>1</v>
       </c>
       <c r="HU5">
-        <v>3900</v>
+        <v>2500</v>
       </c>
       <c r="HV5">
-        <v>3900</v>
+        <v>2500</v>
       </c>
       <c r="HW5">
         <v>0.95</v>
@@ -4935,10 +4872,10 @@
         <v>1</v>
       </c>
       <c r="ID5">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE5">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF5">
         <v>0.95</v>
@@ -4950,43 +4887,43 @@
         <v>303</v>
       </c>
       <c r="II5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK5">
         <v>120</v>
       </c>
       <c r="IL5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM5">
         <v>120</v>
       </c>
       <c r="IN5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO5">
         <v>86400</v>
       </c>
       <c r="IP5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ5">
         <v>120</v>
       </c>
       <c r="IR5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS5">
         <v>120</v>
       </c>
       <c r="IT5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU5">
-        <v>86400</v>
+        <v>57600</v>
       </c>
       <c r="IV5">
         <v>1</v>
@@ -5007,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="JB5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC5" t="s">
         <v>298</v>
@@ -5019,7 +4956,7 @@
         <v>298</v>
       </c>
       <c r="JF5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG5">
         <v>86400</v>
@@ -5039,10 +4976,10 @@
         <v>272</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -5051,7 +4988,7 @@
         <v>2.6</v>
       </c>
       <c r="J6">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -5063,10 +5000,10 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>4536000</v>
+        <v>3125000</v>
       </c>
       <c r="O6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P6" t="s">
         <v>285</v>
@@ -5192,7 +5129,7 @@
         <v>1</v>
       </c>
       <c r="BG6">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH6" t="s">
         <v>294</v>
@@ -5312,24 +5249,9 @@
         <v>3</v>
       </c>
       <c r="CX6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY6">
-        <v>1</v>
-      </c>
-      <c r="CZ6">
-        <v>7200</v>
-      </c>
-      <c r="DA6" t="s">
-        <v>300</v>
-      </c>
-      <c r="DB6">
-        <v>-20</v>
-      </c>
-      <c r="DC6">
-        <v>50</v>
-      </c>
-      <c r="DD6" t="b">
         <v>0</v>
       </c>
       <c r="DE6" t="s">
@@ -5522,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="FV6">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW6" t="s">
         <v>304</v>
@@ -5588,22 +5510,22 @@
         <v>1</v>
       </c>
       <c r="GR6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="GS6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="GT6">
-        <v>75000</v>
+        <v>50000</v>
       </c>
       <c r="GU6">
         <v>7200</v>
       </c>
       <c r="GV6">
-        <v>11000</v>
+        <v>7200</v>
       </c>
       <c r="GW6">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="GX6">
         <v>0.9</v>
@@ -5617,8 +5539,35 @@
       <c r="HA6" t="b">
         <v>0</v>
       </c>
+      <c r="HB6" t="s">
+        <v>311</v>
+      </c>
+      <c r="HC6">
+        <v>100000</v>
+      </c>
+      <c r="HD6">
+        <v>11000</v>
+      </c>
+      <c r="HE6">
+        <v>22000</v>
+      </c>
+      <c r="HF6">
+        <v>200000</v>
+      </c>
+      <c r="HG6">
+        <v>0.9</v>
+      </c>
+      <c r="HH6">
+        <v>0.8</v>
+      </c>
+      <c r="HI6" t="b">
+        <v>0</v>
+      </c>
+      <c r="HJ6" t="b">
+        <v>0</v>
+      </c>
       <c r="HK6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL6">
         <v>0.05</v>
@@ -5633,36 +5582,18 @@
         <v>8.5</v>
       </c>
       <c r="HP6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR6" t="s">
         <v>303</v>
       </c>
       <c r="HS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT6">
-        <v>1</v>
-      </c>
-      <c r="HU6">
-        <v>4500</v>
-      </c>
-      <c r="HV6">
-        <v>4500</v>
-      </c>
-      <c r="HW6">
-        <v>0.95</v>
-      </c>
-      <c r="HX6">
-        <v>0.1</v>
-      </c>
-      <c r="HY6" t="b">
-        <v>0</v>
-      </c>
-      <c r="HZ6" t="b">
         <v>0</v>
       </c>
       <c r="IA6" t="s">
@@ -5675,10 +5606,10 @@
         <v>1</v>
       </c>
       <c r="ID6">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE6">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF6">
         <v>0.95</v>
@@ -5690,43 +5621,43 @@
         <v>303</v>
       </c>
       <c r="II6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK6">
         <v>120</v>
       </c>
       <c r="IL6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM6">
         <v>120</v>
       </c>
       <c r="IN6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO6">
         <v>86400</v>
       </c>
       <c r="IP6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ6">
         <v>120</v>
       </c>
       <c r="IR6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS6">
         <v>120</v>
       </c>
       <c r="IT6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU6">
-        <v>72000</v>
+        <v>57600</v>
       </c>
       <c r="IV6">
         <v>1</v>
@@ -5747,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="JB6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC6" t="s">
         <v>298</v>
@@ -5759,7 +5690,7 @@
         <v>298</v>
       </c>
       <c r="JF6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG6">
         <v>86400</v>
@@ -5779,10 +5710,10 @@
         <v>273</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -5791,7 +5722,7 @@
         <v>2.6</v>
       </c>
       <c r="J7">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -5803,10 +5734,10 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>3863000</v>
+        <v>3564000</v>
       </c>
       <c r="O7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="P7" t="s">
         <v>285</v>
@@ -5932,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="BG7">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH7" t="s">
         <v>295</v>
@@ -6058,16 +5989,16 @@
         <v>1</v>
       </c>
       <c r="CZ7">
-        <v>4700</v>
+        <v>5200</v>
       </c>
       <c r="DA7" t="s">
         <v>300</v>
       </c>
       <c r="DB7">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="DC7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="DD7" t="b">
         <v>0</v>
@@ -6262,10 +6193,10 @@
         <v>1</v>
       </c>
       <c r="FV7">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="FX7" t="s">
         <v>298</v>
@@ -6325,13 +6256,40 @@
         <v>303</v>
       </c>
       <c r="GQ7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR7">
+        <v>1</v>
+      </c>
+      <c r="GS7" t="s">
+        <v>308</v>
+      </c>
+      <c r="GT7">
+        <v>50000</v>
+      </c>
+      <c r="GU7">
+        <v>7200</v>
+      </c>
+      <c r="GV7">
+        <v>7200</v>
+      </c>
+      <c r="GW7">
+        <v>50000</v>
+      </c>
+      <c r="GX7">
+        <v>0.9</v>
+      </c>
+      <c r="GY7">
+        <v>0.8</v>
+      </c>
+      <c r="GZ7" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA7" t="b">
         <v>0</v>
       </c>
       <c r="HK7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL7">
         <v>0.05</v>
@@ -6346,10 +6304,10 @@
         <v>8.5</v>
       </c>
       <c r="HP7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR7" t="s">
         <v>303</v>
@@ -6361,10 +6319,10 @@
         <v>1</v>
       </c>
       <c r="HU7">
-        <v>3900</v>
+        <v>3600</v>
       </c>
       <c r="HV7">
-        <v>3900</v>
+        <v>3600</v>
       </c>
       <c r="HW7">
         <v>0.95</v>
@@ -6388,10 +6346,10 @@
         <v>1</v>
       </c>
       <c r="ID7">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE7">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF7">
         <v>0.95</v>
@@ -6403,40 +6361,40 @@
         <v>303</v>
       </c>
       <c r="II7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK7">
         <v>120</v>
       </c>
       <c r="IL7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM7">
         <v>120</v>
       </c>
       <c r="IN7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO7">
         <v>86400</v>
       </c>
       <c r="IP7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ7">
         <v>120</v>
       </c>
       <c r="IR7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS7">
         <v>120</v>
       </c>
       <c r="IT7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU7">
         <v>72000</v>
@@ -6460,7 +6418,7 @@
         <v>1</v>
       </c>
       <c r="JB7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC7" t="s">
         <v>298</v>
@@ -6472,7 +6430,7 @@
         <v>298</v>
       </c>
       <c r="JF7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG7">
         <v>86400</v>
@@ -6516,10 +6474,10 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>3863000</v>
+        <v>5527000</v>
       </c>
       <c r="O8" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="P8" t="s">
         <v>285</v>
@@ -6648,10 +6606,10 @@
         <v>5500000</v>
       </c>
       <c r="BH8" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="BI8">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="BJ8" t="s">
         <v>298</v>
@@ -6963,7 +6921,7 @@
         <v>2800</v>
       </c>
       <c r="FW8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="FX8" t="s">
         <v>298</v>
@@ -7023,13 +6981,40 @@
         <v>303</v>
       </c>
       <c r="GQ8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR8">
+        <v>1</v>
+      </c>
+      <c r="GS8" t="s">
+        <v>309</v>
+      </c>
+      <c r="GT8">
+        <v>100000</v>
+      </c>
+      <c r="GU8">
+        <v>11000</v>
+      </c>
+      <c r="GV8">
+        <v>22000</v>
+      </c>
+      <c r="GW8">
+        <v>200000</v>
+      </c>
+      <c r="GX8">
+        <v>0.9</v>
+      </c>
+      <c r="GY8">
+        <v>0.8</v>
+      </c>
+      <c r="GZ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA8" t="b">
         <v>0</v>
       </c>
       <c r="HK8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL8">
         <v>0.05</v>
@@ -7044,10 +7029,10 @@
         <v>8.5</v>
       </c>
       <c r="HP8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR8" t="s">
         <v>303</v>
@@ -7083,43 +7068,43 @@
         <v>303</v>
       </c>
       <c r="II8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK8">
         <v>120</v>
       </c>
       <c r="IL8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM8">
         <v>120</v>
       </c>
       <c r="IN8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO8">
         <v>86400</v>
       </c>
       <c r="IP8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ8">
         <v>120</v>
       </c>
       <c r="IR8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS8">
         <v>120</v>
       </c>
       <c r="IT8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU8">
-        <v>86400</v>
+        <v>72000</v>
       </c>
       <c r="IV8">
         <v>1</v>
@@ -7140,7 +7125,7 @@
         <v>1</v>
       </c>
       <c r="JB8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC8" t="s">
         <v>298</v>
@@ -7152,7 +7137,7 @@
         <v>298</v>
       </c>
       <c r="JF8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG8">
         <v>86400</v>
@@ -7172,10 +7157,10 @@
         <v>275</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -7184,7 +7169,7 @@
         <v>2.6</v>
       </c>
       <c r="J9">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -7196,7 +7181,7 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>3564000</v>
+        <v>5527000</v>
       </c>
       <c r="O9" t="s">
         <v>283</v>
@@ -7325,7 +7310,7 @@
         <v>1</v>
       </c>
       <c r="BG9">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH9" t="s">
         <v>296</v>
@@ -7451,7 +7436,7 @@
         <v>1</v>
       </c>
       <c r="CZ9">
-        <v>5600</v>
+        <v>8100</v>
       </c>
       <c r="DA9" t="s">
         <v>300</v>
@@ -7655,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="FV9">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW9" t="s">
         <v>304</v>
@@ -7718,13 +7703,40 @@
         <v>303</v>
       </c>
       <c r="GQ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR9">
+        <v>1</v>
+      </c>
+      <c r="GS9" t="s">
+        <v>310</v>
+      </c>
+      <c r="GT9">
+        <v>75000</v>
+      </c>
+      <c r="GU9">
+        <v>7200</v>
+      </c>
+      <c r="GV9">
+        <v>11000</v>
+      </c>
+      <c r="GW9">
+        <v>100000</v>
+      </c>
+      <c r="GX9">
+        <v>0.9</v>
+      </c>
+      <c r="GY9">
+        <v>0.8</v>
+      </c>
+      <c r="GZ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA9" t="b">
         <v>0</v>
       </c>
       <c r="HK9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL9">
         <v>0.05</v>
@@ -7739,18 +7751,36 @@
         <v>8.5</v>
       </c>
       <c r="HP9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR9" t="s">
         <v>303</v>
       </c>
       <c r="HS9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HT9">
+        <v>1</v>
+      </c>
+      <c r="HU9">
+        <v>5500</v>
+      </c>
+      <c r="HV9">
+        <v>5500</v>
+      </c>
+      <c r="HW9">
+        <v>0.95</v>
+      </c>
+      <c r="HX9">
+        <v>0.1</v>
+      </c>
+      <c r="HY9" t="b">
+        <v>0</v>
+      </c>
+      <c r="HZ9" t="b">
         <v>0</v>
       </c>
       <c r="IA9" t="s">
@@ -7763,10 +7793,10 @@
         <v>1</v>
       </c>
       <c r="ID9">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE9">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF9">
         <v>0.95</v>
@@ -7778,43 +7808,43 @@
         <v>303</v>
       </c>
       <c r="II9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK9">
         <v>120</v>
       </c>
       <c r="IL9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM9">
         <v>120</v>
       </c>
       <c r="IN9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO9">
         <v>86400</v>
       </c>
       <c r="IP9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ9">
         <v>120</v>
       </c>
       <c r="IR9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS9">
         <v>120</v>
       </c>
       <c r="IT9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU9">
-        <v>86400</v>
+        <v>57600</v>
       </c>
       <c r="IV9">
         <v>1</v>
@@ -7835,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="JB9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC9" t="s">
         <v>298</v>
@@ -7847,7 +7877,7 @@
         <v>298</v>
       </c>
       <c r="JF9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG9">
         <v>86400</v>
@@ -7891,10 +7921,10 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>3125000</v>
+        <v>4402000</v>
       </c>
       <c r="O10" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="P10" t="s">
         <v>285</v>
@@ -8023,10 +8053,10 @@
         <v>19500000</v>
       </c>
       <c r="BH10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="BI10">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="BJ10" t="s">
         <v>298</v>
@@ -8146,16 +8176,16 @@
         <v>1</v>
       </c>
       <c r="CZ10">
-        <v>4900</v>
+        <v>7400</v>
       </c>
       <c r="DA10" t="s">
         <v>300</v>
       </c>
       <c r="DB10">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="DC10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="DD10" t="b">
         <v>0</v>
@@ -8353,7 +8383,7 @@
         <v>9800</v>
       </c>
       <c r="FW10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="FX10" t="s">
         <v>298</v>
@@ -8419,7 +8449,7 @@
         <v>0</v>
       </c>
       <c r="HK10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL10">
         <v>0.05</v>
@@ -8434,10 +8464,10 @@
         <v>8.5</v>
       </c>
       <c r="HP10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR10" t="s">
         <v>303</v>
@@ -8449,10 +8479,10 @@
         <v>1</v>
       </c>
       <c r="HU10">
-        <v>3100</v>
+        <v>4400</v>
       </c>
       <c r="HV10">
-        <v>3100</v>
+        <v>4400</v>
       </c>
       <c r="HW10">
         <v>0.95</v>
@@ -8491,40 +8521,40 @@
         <v>303</v>
       </c>
       <c r="II10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK10">
         <v>120</v>
       </c>
       <c r="IL10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM10">
         <v>120</v>
       </c>
       <c r="IN10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO10">
         <v>86400</v>
       </c>
       <c r="IP10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ10">
         <v>120</v>
       </c>
       <c r="IR10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS10">
         <v>120</v>
       </c>
       <c r="IT10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU10">
         <v>86400</v>
@@ -8548,7 +8578,7 @@
         <v>1</v>
       </c>
       <c r="JB10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC10" t="s">
         <v>298</v>
@@ -8560,7 +8590,7 @@
         <v>298</v>
       </c>
       <c r="JF10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG10">
         <v>86400</v>
@@ -8580,10 +8610,10 @@
         <v>277</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -8592,7 +8622,7 @@
         <v>2.6</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -8604,10 +8634,10 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>5527000</v>
+        <v>3863000</v>
       </c>
       <c r="O11" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="P11" t="s">
         <v>285</v>
@@ -8733,10 +8763,10 @@
         <v>1</v>
       </c>
       <c r="BG11">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH11" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="BI11">
         <v>55</v>
@@ -8859,7 +8889,7 @@
         <v>1</v>
       </c>
       <c r="CZ11">
-        <v>7200</v>
+        <v>5600</v>
       </c>
       <c r="DA11" t="s">
         <v>300</v>
@@ -9063,10 +9093,10 @@
         <v>1</v>
       </c>
       <c r="FV11">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="FX11" t="s">
         <v>298</v>
@@ -9126,67 +9156,13 @@
         <v>303</v>
       </c>
       <c r="GQ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR11">
-        <v>2</v>
-      </c>
-      <c r="GS11" t="s">
-        <v>310</v>
-      </c>
-      <c r="GT11">
-        <v>50000</v>
-      </c>
-      <c r="GU11">
-        <v>7200</v>
-      </c>
-      <c r="GV11">
-        <v>7200</v>
-      </c>
-      <c r="GW11">
-        <v>50000</v>
-      </c>
-      <c r="GX11">
-        <v>0.9</v>
-      </c>
-      <c r="GY11">
-        <v>0.8</v>
-      </c>
-      <c r="GZ11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HB11" t="s">
-        <v>308</v>
-      </c>
-      <c r="HC11">
-        <v>75000</v>
-      </c>
-      <c r="HD11">
-        <v>7200</v>
-      </c>
-      <c r="HE11">
-        <v>11000</v>
-      </c>
-      <c r="HF11">
-        <v>100000</v>
-      </c>
-      <c r="HG11">
-        <v>0.9</v>
-      </c>
-      <c r="HH11">
-        <v>0.8</v>
-      </c>
-      <c r="HI11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HJ11" t="b">
         <v>0</v>
       </c>
       <c r="HK11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL11">
         <v>0.05</v>
@@ -9201,10 +9177,10 @@
         <v>8.5</v>
       </c>
       <c r="HP11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR11" t="s">
         <v>303</v>
@@ -9216,10 +9192,10 @@
         <v>1</v>
       </c>
       <c r="HU11">
-        <v>5500</v>
+        <v>3900</v>
       </c>
       <c r="HV11">
-        <v>5500</v>
+        <v>3900</v>
       </c>
       <c r="HW11">
         <v>0.95</v>
@@ -9243,10 +9219,10 @@
         <v>1</v>
       </c>
       <c r="ID11">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE11">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF11">
         <v>0.95</v>
@@ -9258,43 +9234,43 @@
         <v>303</v>
       </c>
       <c r="II11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK11">
         <v>120</v>
       </c>
       <c r="IL11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM11">
         <v>120</v>
       </c>
       <c r="IN11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO11">
         <v>86400</v>
       </c>
       <c r="IP11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ11">
         <v>120</v>
       </c>
       <c r="IR11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS11">
         <v>120</v>
       </c>
       <c r="IT11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU11">
-        <v>57600</v>
+        <v>72000</v>
       </c>
       <c r="IV11">
         <v>1</v>
@@ -9315,7 +9291,7 @@
         <v>1</v>
       </c>
       <c r="JB11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC11" t="s">
         <v>298</v>
@@ -9327,7 +9303,7 @@
         <v>298</v>
       </c>
       <c r="JF11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG11">
         <v>86400</v>

</xml_diff>

<commit_message>
cache the whole general data (including weather data)
This needs to be done in order to avoid reading it over and over again
which needs lots of time and memory.
</commit_message>
<xml_diff>
--- a/02_config/example_single_market/agents.xlsx
+++ b/02_config/example_single_market/agents.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="319">
   <si>
     <t>general/agent_id</t>
   </si>
@@ -820,57 +820,57 @@
     <t>ems/fcasts/update</t>
   </si>
   <si>
-    <t>BsIKeyrf1lj3rVO</t>
-  </si>
-  <si>
-    <t>8f3vvlIRj9ICt8O</t>
-  </si>
-  <si>
-    <t>T0trImFXXGMgP9I</t>
-  </si>
-  <si>
-    <t>bZHXZoNjVVbyhNo</t>
-  </si>
-  <si>
-    <t>79O1mruFbVgykmF</t>
-  </si>
-  <si>
-    <t>EVzNaAJab8rA3Go</t>
-  </si>
-  <si>
-    <t>QFcbDCphvAGIikn</t>
-  </si>
-  <si>
-    <t>N0HOa2ZKJcz12gC</t>
-  </si>
-  <si>
-    <t>Ts9tuWCg09uwsSa</t>
-  </si>
-  <si>
-    <t>spIQTuoMuglwLsn</t>
-  </si>
-  <si>
-    <t>hh_2959_0.csv</t>
+    <t>7RoMKhKPykXrFxN</t>
+  </si>
+  <si>
+    <t>ryYqphAYH66rqBR</t>
+  </si>
+  <si>
+    <t>9EzYHF2KmClcoSH</t>
+  </si>
+  <si>
+    <t>To06tKG30CoaBBZ</t>
+  </si>
+  <si>
+    <t>ci3ggclTDIuxx0J</t>
+  </si>
+  <si>
+    <t>8HAaGxfdIuOYpoE</t>
+  </si>
+  <si>
+    <t>li0yQQQ2eFSuKVB</t>
+  </si>
+  <si>
+    <t>S3jFOl27BE4LplR</t>
+  </si>
+  <si>
+    <t>YawQtd5fYkC08f3</t>
+  </si>
+  <si>
+    <t>fkJkOc4Pri4u6sg</t>
+  </si>
+  <si>
+    <t>hh_2532_0.csv</t>
+  </si>
+  <si>
+    <t>hh_4402_0.csv</t>
+  </si>
+  <si>
+    <t>hh_4536_0.csv</t>
+  </si>
+  <si>
+    <t>hh_3125_0.csv</t>
+  </si>
+  <si>
+    <t>hh_3564_0.csv</t>
   </si>
   <si>
     <t>hh_5527_0.csv</t>
   </si>
   <si>
-    <t>hh_2896_0.csv</t>
-  </si>
-  <si>
     <t>hh_3863_0.csv</t>
   </si>
   <si>
-    <t>hh_4536_0.csv</t>
-  </si>
-  <si>
-    <t>hh_3564_0.csv</t>
-  </si>
-  <si>
-    <t>hh_3125_0.csv</t>
-  </si>
-  <si>
     <t>perfect</t>
   </si>
   <si>
@@ -886,28 +886,28 @@
     <t>rfr</t>
   </si>
   <si>
-    <t>heat_2959_0.csv</t>
+    <t>heat_gen_4_pu.csv</t>
+  </si>
+  <si>
+    <t>heat_4402_0.csv</t>
+  </si>
+  <si>
+    <t>heat_gen_0_pu.csv</t>
+  </si>
+  <si>
+    <t>heat_2532_0.csv</t>
+  </si>
+  <si>
+    <t>heat_3125_0.csv</t>
+  </si>
+  <si>
+    <t>heat_3564_0.csv</t>
   </si>
   <si>
     <t>heat_5527_0.csv</t>
   </si>
   <si>
-    <t>heat_gen_0_pu.csv</t>
-  </si>
-  <si>
-    <t>heat_3863_0.csv</t>
-  </si>
-  <si>
-    <t>heat_4536_0.csv</t>
-  </si>
-  <si>
-    <t>heat_gen_5_pu.csv</t>
-  </si>
-  <si>
-    <t>heat_3564_0.csv</t>
-  </si>
-  <si>
-    <t>heat_3125_0.csv</t>
+    <t>heat_gen_1_pu.csv</t>
   </si>
   <si>
     <t>naive</t>
@@ -934,19 +934,22 @@
     <t>hp_DAIKIN Europe_ground.json</t>
   </si>
   <si>
+    <t>ev_freetime_3.csv</t>
+  </si>
+  <si>
     <t>ev_fulltime_48.csv</t>
   </si>
   <si>
-    <t>ev_freetime_1.csv</t>
-  </si>
-  <si>
-    <t>ev_fulltime_47.csv</t>
-  </si>
-  <si>
-    <t>ev_freetime_3.csv</t>
-  </si>
-  <si>
-    <t>ev_fulltime_44.csv</t>
+    <t>ev_freetime_2.csv</t>
+  </si>
+  <si>
+    <t>ev_fulltime_42.csv</t>
+  </si>
+  <si>
+    <t>ev_parttime_88.csv</t>
+  </si>
+  <si>
+    <t>ev_fulltime_45.csv</t>
   </si>
   <si>
     <t>min_soc</t>
@@ -2145,10 +2148,10 @@
         <v>268</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H2">
         <v>2</v>
@@ -2157,7 +2160,7 @@
         <v>2.6</v>
       </c>
       <c r="J2">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2169,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>2959000</v>
+        <v>2532000</v>
       </c>
       <c r="O2" t="s">
         <v>278</v>
@@ -2298,7 +2301,7 @@
         <v>1</v>
       </c>
       <c r="BG2">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH2" t="s">
         <v>290</v>
@@ -2424,7 +2427,7 @@
         <v>1</v>
       </c>
       <c r="CZ2">
-        <v>5100</v>
+        <v>4100</v>
       </c>
       <c r="DA2" t="s">
         <v>300</v>
@@ -2628,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="FV2">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW2" t="s">
         <v>304</v>
@@ -2691,67 +2694,13 @@
         <v>303</v>
       </c>
       <c r="GQ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR2">
-        <v>2</v>
-      </c>
-      <c r="GS2" t="s">
-        <v>306</v>
-      </c>
-      <c r="GT2">
-        <v>50000</v>
-      </c>
-      <c r="GU2">
-        <v>7200</v>
-      </c>
-      <c r="GV2">
-        <v>7200</v>
-      </c>
-      <c r="GW2">
-        <v>50000</v>
-      </c>
-      <c r="GX2">
-        <v>0.9</v>
-      </c>
-      <c r="GY2">
-        <v>0.8</v>
-      </c>
-      <c r="GZ2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HB2" t="s">
-        <v>308</v>
-      </c>
-      <c r="HC2">
-        <v>50000</v>
-      </c>
-      <c r="HD2">
-        <v>7200</v>
-      </c>
-      <c r="HE2">
-        <v>7200</v>
-      </c>
-      <c r="HF2">
-        <v>50000</v>
-      </c>
-      <c r="HG2">
-        <v>0.9</v>
-      </c>
-      <c r="HH2">
-        <v>0.8</v>
-      </c>
-      <c r="HI2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HJ2" t="b">
         <v>0</v>
       </c>
       <c r="HK2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL2">
         <v>0.05</v>
@@ -2766,36 +2715,18 @@
         <v>8.5</v>
       </c>
       <c r="HP2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR2" t="s">
         <v>303</v>
       </c>
       <c r="HS2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT2">
-        <v>1</v>
-      </c>
-      <c r="HU2">
-        <v>3000</v>
-      </c>
-      <c r="HV2">
-        <v>3000</v>
-      </c>
-      <c r="HW2">
-        <v>0.95</v>
-      </c>
-      <c r="HX2">
-        <v>0.1</v>
-      </c>
-      <c r="HY2" t="b">
-        <v>0</v>
-      </c>
-      <c r="HZ2" t="b">
         <v>0</v>
       </c>
       <c r="IA2" t="s">
@@ -2808,10 +2739,10 @@
         <v>1</v>
       </c>
       <c r="ID2">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE2">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF2">
         <v>0.95</v>
@@ -2823,43 +2754,43 @@
         <v>303</v>
       </c>
       <c r="II2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK2">
         <v>120</v>
       </c>
       <c r="IL2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM2">
         <v>120</v>
       </c>
       <c r="IN2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO2">
         <v>86400</v>
       </c>
       <c r="IP2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ2">
         <v>120</v>
       </c>
       <c r="IR2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS2">
         <v>120</v>
       </c>
       <c r="IT2" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU2">
-        <v>43200</v>
+        <v>57600</v>
       </c>
       <c r="IV2">
         <v>1</v>
@@ -2880,7 +2811,7 @@
         <v>1</v>
       </c>
       <c r="JB2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC2" t="s">
         <v>298</v>
@@ -2892,7 +2823,7 @@
         <v>298</v>
       </c>
       <c r="JF2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG2">
         <v>86400</v>
@@ -2912,10 +2843,10 @@
         <v>269</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -2924,7 +2855,7 @@
         <v>2.6</v>
       </c>
       <c r="J3">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -2936,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>5527000</v>
+        <v>4402000</v>
       </c>
       <c r="O3" t="s">
         <v>279</v>
@@ -3065,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="BG3">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH3" t="s">
         <v>291</v>
@@ -3380,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="FV3">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW3" t="s">
         <v>304</v>
@@ -3449,19 +3380,19 @@
         <v>1</v>
       </c>
       <c r="GS3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="GT3">
+        <v>75000</v>
+      </c>
+      <c r="GU3">
+        <v>7200</v>
+      </c>
+      <c r="GV3">
+        <v>11000</v>
+      </c>
+      <c r="GW3">
         <v>100000</v>
-      </c>
-      <c r="GU3">
-        <v>11000</v>
-      </c>
-      <c r="GV3">
-        <v>22000</v>
-      </c>
-      <c r="GW3">
-        <v>200000</v>
       </c>
       <c r="GX3">
         <v>0.9</v>
@@ -3476,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="HK3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL3">
         <v>0.05</v>
@@ -3491,10 +3422,10 @@
         <v>8.5</v>
       </c>
       <c r="HP3" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ3" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR3" t="s">
         <v>303</v>
@@ -3515,10 +3446,10 @@
         <v>1</v>
       </c>
       <c r="ID3">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE3">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF3">
         <v>0.95</v>
@@ -3530,43 +3461,43 @@
         <v>303</v>
       </c>
       <c r="II3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK3">
         <v>120</v>
       </c>
       <c r="IL3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM3">
         <v>120</v>
       </c>
       <c r="IN3" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO3">
         <v>86400</v>
       </c>
       <c r="IP3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ3">
         <v>120</v>
       </c>
       <c r="IR3" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS3">
         <v>120</v>
       </c>
       <c r="IT3" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU3">
-        <v>57600</v>
+        <v>86400</v>
       </c>
       <c r="IV3">
         <v>1</v>
@@ -3587,7 +3518,7 @@
         <v>1</v>
       </c>
       <c r="JB3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC3" t="s">
         <v>298</v>
@@ -3599,7 +3530,7 @@
         <v>298</v>
       </c>
       <c r="JF3" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG3">
         <v>86400</v>
@@ -3619,10 +3550,10 @@
         <v>270</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H4">
         <v>2</v>
@@ -3631,7 +3562,7 @@
         <v>2.6</v>
       </c>
       <c r="J4">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -3643,7 +3574,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>2896000</v>
+        <v>4536000</v>
       </c>
       <c r="O4" t="s">
         <v>280</v>
@@ -3772,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="BG4">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH4" t="s">
         <v>292</v>
@@ -3892,9 +3823,24 @@
         <v>3</v>
       </c>
       <c r="CX4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CY4">
+        <v>1</v>
+      </c>
+      <c r="CZ4">
+        <v>7600</v>
+      </c>
+      <c r="DA4" t="s">
+        <v>300</v>
+      </c>
+      <c r="DB4">
+        <v>0</v>
+      </c>
+      <c r="DC4">
+        <v>40</v>
+      </c>
+      <c r="DD4" t="b">
         <v>0</v>
       </c>
       <c r="DE4" t="s">
@@ -4087,7 +4033,7 @@
         <v>1</v>
       </c>
       <c r="FV4">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW4" t="s">
         <v>304</v>
@@ -4150,40 +4096,13 @@
         <v>303</v>
       </c>
       <c r="GQ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR4">
-        <v>1</v>
-      </c>
-      <c r="GS4" t="s">
-        <v>308</v>
-      </c>
-      <c r="GT4">
-        <v>75000</v>
-      </c>
-      <c r="GU4">
-        <v>7200</v>
-      </c>
-      <c r="GV4">
-        <v>11000</v>
-      </c>
-      <c r="GW4">
-        <v>100000</v>
-      </c>
-      <c r="GX4">
-        <v>0.9</v>
-      </c>
-      <c r="GY4">
-        <v>0.8</v>
-      </c>
-      <c r="GZ4" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA4" t="b">
         <v>0</v>
       </c>
       <c r="HK4" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL4">
         <v>0.05</v>
@@ -4198,18 +4117,36 @@
         <v>8.5</v>
       </c>
       <c r="HP4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR4" t="s">
         <v>303</v>
       </c>
       <c r="HS4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HT4">
+        <v>1</v>
+      </c>
+      <c r="HU4">
+        <v>4500</v>
+      </c>
+      <c r="HV4">
+        <v>4500</v>
+      </c>
+      <c r="HW4">
+        <v>0.95</v>
+      </c>
+      <c r="HX4">
+        <v>0.1</v>
+      </c>
+      <c r="HY4" t="b">
+        <v>0</v>
+      </c>
+      <c r="HZ4" t="b">
         <v>0</v>
       </c>
       <c r="IA4" t="s">
@@ -4222,10 +4159,10 @@
         <v>1</v>
       </c>
       <c r="ID4">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE4">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF4">
         <v>0.95</v>
@@ -4237,40 +4174,40 @@
         <v>303</v>
       </c>
       <c r="II4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK4">
         <v>120</v>
       </c>
       <c r="IL4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM4">
         <v>120</v>
       </c>
       <c r="IN4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO4">
         <v>86400</v>
       </c>
       <c r="IP4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ4">
         <v>120</v>
       </c>
       <c r="IR4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS4">
         <v>120</v>
       </c>
       <c r="IT4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU4">
         <v>57600</v>
@@ -4294,7 +4231,7 @@
         <v>1</v>
       </c>
       <c r="JB4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC4" t="s">
         <v>298</v>
@@ -4306,7 +4243,7 @@
         <v>298</v>
       </c>
       <c r="JF4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG4">
         <v>86400</v>
@@ -4326,10 +4263,10 @@
         <v>271</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -4338,7 +4275,7 @@
         <v>2.6</v>
       </c>
       <c r="J5">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -4350,10 +4287,10 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>3863000</v>
+        <v>2532000</v>
       </c>
       <c r="O5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="P5" t="s">
         <v>285</v>
@@ -4479,7 +4416,7 @@
         <v>1</v>
       </c>
       <c r="BG5">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH5" t="s">
         <v>293</v>
@@ -4605,16 +4542,16 @@
         <v>1</v>
       </c>
       <c r="CZ5">
-        <v>5700</v>
+        <v>3800</v>
       </c>
       <c r="DA5" t="s">
         <v>300</v>
       </c>
       <c r="DB5">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="DC5">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="DD5" t="b">
         <v>0</v>
@@ -4809,7 +4746,7 @@
         <v>1</v>
       </c>
       <c r="FV5">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW5" t="s">
         <v>304</v>
@@ -4878,7 +4815,7 @@
         <v>0</v>
       </c>
       <c r="HK5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL5">
         <v>0.05</v>
@@ -4893,10 +4830,10 @@
         <v>8.5</v>
       </c>
       <c r="HP5" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR5" t="s">
         <v>303</v>
@@ -4908,10 +4845,10 @@
         <v>1</v>
       </c>
       <c r="HU5">
-        <v>3900</v>
+        <v>2500</v>
       </c>
       <c r="HV5">
-        <v>3900</v>
+        <v>2500</v>
       </c>
       <c r="HW5">
         <v>0.95</v>
@@ -4935,10 +4872,10 @@
         <v>1</v>
       </c>
       <c r="ID5">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE5">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF5">
         <v>0.95</v>
@@ -4950,43 +4887,43 @@
         <v>303</v>
       </c>
       <c r="II5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK5">
         <v>120</v>
       </c>
       <c r="IL5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM5">
         <v>120</v>
       </c>
       <c r="IN5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO5">
         <v>86400</v>
       </c>
       <c r="IP5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ5">
         <v>120</v>
       </c>
       <c r="IR5" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS5">
         <v>120</v>
       </c>
       <c r="IT5" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU5">
-        <v>86400</v>
+        <v>57600</v>
       </c>
       <c r="IV5">
         <v>1</v>
@@ -5007,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="JB5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC5" t="s">
         <v>298</v>
@@ -5019,7 +4956,7 @@
         <v>298</v>
       </c>
       <c r="JF5" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG5">
         <v>86400</v>
@@ -5039,10 +4976,10 @@
         <v>272</v>
       </c>
       <c r="F6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -5051,7 +4988,7 @@
         <v>2.6</v>
       </c>
       <c r="J6">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -5063,10 +5000,10 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>4536000</v>
+        <v>3125000</v>
       </c>
       <c r="O6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P6" t="s">
         <v>285</v>
@@ -5192,7 +5129,7 @@
         <v>1</v>
       </c>
       <c r="BG6">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH6" t="s">
         <v>294</v>
@@ -5312,24 +5249,9 @@
         <v>3</v>
       </c>
       <c r="CX6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY6">
-        <v>1</v>
-      </c>
-      <c r="CZ6">
-        <v>7200</v>
-      </c>
-      <c r="DA6" t="s">
-        <v>300</v>
-      </c>
-      <c r="DB6">
-        <v>-20</v>
-      </c>
-      <c r="DC6">
-        <v>50</v>
-      </c>
-      <c r="DD6" t="b">
         <v>0</v>
       </c>
       <c r="DE6" t="s">
@@ -5522,7 +5444,7 @@
         <v>1</v>
       </c>
       <c r="FV6">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW6" t="s">
         <v>304</v>
@@ -5588,22 +5510,22 @@
         <v>1</v>
       </c>
       <c r="GR6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="GS6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="GT6">
-        <v>75000</v>
+        <v>50000</v>
       </c>
       <c r="GU6">
         <v>7200</v>
       </c>
       <c r="GV6">
-        <v>11000</v>
+        <v>7200</v>
       </c>
       <c r="GW6">
-        <v>100000</v>
+        <v>50000</v>
       </c>
       <c r="GX6">
         <v>0.9</v>
@@ -5617,8 +5539,35 @@
       <c r="HA6" t="b">
         <v>0</v>
       </c>
+      <c r="HB6" t="s">
+        <v>311</v>
+      </c>
+      <c r="HC6">
+        <v>100000</v>
+      </c>
+      <c r="HD6">
+        <v>11000</v>
+      </c>
+      <c r="HE6">
+        <v>22000</v>
+      </c>
+      <c r="HF6">
+        <v>200000</v>
+      </c>
+      <c r="HG6">
+        <v>0.9</v>
+      </c>
+      <c r="HH6">
+        <v>0.8</v>
+      </c>
+      <c r="HI6" t="b">
+        <v>0</v>
+      </c>
+      <c r="HJ6" t="b">
+        <v>0</v>
+      </c>
       <c r="HK6" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL6">
         <v>0.05</v>
@@ -5633,36 +5582,18 @@
         <v>8.5</v>
       </c>
       <c r="HP6" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ6" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR6" t="s">
         <v>303</v>
       </c>
       <c r="HS6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="HT6">
-        <v>1</v>
-      </c>
-      <c r="HU6">
-        <v>4500</v>
-      </c>
-      <c r="HV6">
-        <v>4500</v>
-      </c>
-      <c r="HW6">
-        <v>0.95</v>
-      </c>
-      <c r="HX6">
-        <v>0.1</v>
-      </c>
-      <c r="HY6" t="b">
-        <v>0</v>
-      </c>
-      <c r="HZ6" t="b">
         <v>0</v>
       </c>
       <c r="IA6" t="s">
@@ -5675,10 +5606,10 @@
         <v>1</v>
       </c>
       <c r="ID6">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE6">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF6">
         <v>0.95</v>
@@ -5690,43 +5621,43 @@
         <v>303</v>
       </c>
       <c r="II6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK6">
         <v>120</v>
       </c>
       <c r="IL6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM6">
         <v>120</v>
       </c>
       <c r="IN6" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO6">
         <v>86400</v>
       </c>
       <c r="IP6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ6">
         <v>120</v>
       </c>
       <c r="IR6" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS6">
         <v>120</v>
       </c>
       <c r="IT6" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU6">
-        <v>72000</v>
+        <v>57600</v>
       </c>
       <c r="IV6">
         <v>1</v>
@@ -5747,7 +5678,7 @@
         <v>1</v>
       </c>
       <c r="JB6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC6" t="s">
         <v>298</v>
@@ -5759,7 +5690,7 @@
         <v>298</v>
       </c>
       <c r="JF6" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG6">
         <v>86400</v>
@@ -5779,10 +5710,10 @@
         <v>273</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="H7">
         <v>2</v>
@@ -5791,7 +5722,7 @@
         <v>2.6</v>
       </c>
       <c r="J7">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -5803,10 +5734,10 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>3863000</v>
+        <v>3564000</v>
       </c>
       <c r="O7" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="P7" t="s">
         <v>285</v>
@@ -5932,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="BG7">
-        <v>5500000</v>
+        <v>19500000</v>
       </c>
       <c r="BH7" t="s">
         <v>295</v>
@@ -6058,16 +5989,16 @@
         <v>1</v>
       </c>
       <c r="CZ7">
-        <v>4700</v>
+        <v>5200</v>
       </c>
       <c r="DA7" t="s">
         <v>300</v>
       </c>
       <c r="DB7">
-        <v>0</v>
+        <v>-20</v>
       </c>
       <c r="DC7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="DD7" t="b">
         <v>0</v>
@@ -6262,10 +6193,10 @@
         <v>1</v>
       </c>
       <c r="FV7">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="FW7" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="FX7" t="s">
         <v>298</v>
@@ -6325,13 +6256,40 @@
         <v>303</v>
       </c>
       <c r="GQ7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR7">
+        <v>1</v>
+      </c>
+      <c r="GS7" t="s">
+        <v>308</v>
+      </c>
+      <c r="GT7">
+        <v>50000</v>
+      </c>
+      <c r="GU7">
+        <v>7200</v>
+      </c>
+      <c r="GV7">
+        <v>7200</v>
+      </c>
+      <c r="GW7">
+        <v>50000</v>
+      </c>
+      <c r="GX7">
+        <v>0.9</v>
+      </c>
+      <c r="GY7">
+        <v>0.8</v>
+      </c>
+      <c r="GZ7" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA7" t="b">
         <v>0</v>
       </c>
       <c r="HK7" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL7">
         <v>0.05</v>
@@ -6346,10 +6304,10 @@
         <v>8.5</v>
       </c>
       <c r="HP7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR7" t="s">
         <v>303</v>
@@ -6361,10 +6319,10 @@
         <v>1</v>
       </c>
       <c r="HU7">
-        <v>3900</v>
+        <v>3600</v>
       </c>
       <c r="HV7">
-        <v>3900</v>
+        <v>3600</v>
       </c>
       <c r="HW7">
         <v>0.95</v>
@@ -6388,10 +6346,10 @@
         <v>1</v>
       </c>
       <c r="ID7">
-        <v>2800</v>
+        <v>9800</v>
       </c>
       <c r="IE7">
-        <v>5500</v>
+        <v>19500</v>
       </c>
       <c r="IF7">
         <v>0.95</v>
@@ -6403,40 +6361,40 @@
         <v>303</v>
       </c>
       <c r="II7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK7">
         <v>120</v>
       </c>
       <c r="IL7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM7">
         <v>120</v>
       </c>
       <c r="IN7" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO7">
         <v>86400</v>
       </c>
       <c r="IP7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ7">
         <v>120</v>
       </c>
       <c r="IR7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS7">
         <v>120</v>
       </c>
       <c r="IT7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU7">
         <v>72000</v>
@@ -6460,7 +6418,7 @@
         <v>1</v>
       </c>
       <c r="JB7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC7" t="s">
         <v>298</v>
@@ -6472,7 +6430,7 @@
         <v>298</v>
       </c>
       <c r="JF7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG7">
         <v>86400</v>
@@ -6516,10 +6474,10 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>3863000</v>
+        <v>5527000</v>
       </c>
       <c r="O8" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="P8" t="s">
         <v>285</v>
@@ -6648,10 +6606,10 @@
         <v>5500000</v>
       </c>
       <c r="BH8" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="BI8">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="BJ8" t="s">
         <v>298</v>
@@ -6963,7 +6921,7 @@
         <v>2800</v>
       </c>
       <c r="FW8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="FX8" t="s">
         <v>298</v>
@@ -7023,13 +6981,40 @@
         <v>303</v>
       </c>
       <c r="GQ8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR8">
+        <v>1</v>
+      </c>
+      <c r="GS8" t="s">
+        <v>309</v>
+      </c>
+      <c r="GT8">
+        <v>100000</v>
+      </c>
+      <c r="GU8">
+        <v>11000</v>
+      </c>
+      <c r="GV8">
+        <v>22000</v>
+      </c>
+      <c r="GW8">
+        <v>200000</v>
+      </c>
+      <c r="GX8">
+        <v>0.9</v>
+      </c>
+      <c r="GY8">
+        <v>0.8</v>
+      </c>
+      <c r="GZ8" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA8" t="b">
         <v>0</v>
       </c>
       <c r="HK8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL8">
         <v>0.05</v>
@@ -7044,10 +7029,10 @@
         <v>8.5</v>
       </c>
       <c r="HP8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR8" t="s">
         <v>303</v>
@@ -7083,43 +7068,43 @@
         <v>303</v>
       </c>
       <c r="II8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK8">
         <v>120</v>
       </c>
       <c r="IL8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM8">
         <v>120</v>
       </c>
       <c r="IN8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO8">
         <v>86400</v>
       </c>
       <c r="IP8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ8">
         <v>120</v>
       </c>
       <c r="IR8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS8">
         <v>120</v>
       </c>
       <c r="IT8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU8">
-        <v>86400</v>
+        <v>72000</v>
       </c>
       <c r="IV8">
         <v>1</v>
@@ -7140,7 +7125,7 @@
         <v>1</v>
       </c>
       <c r="JB8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC8" t="s">
         <v>298</v>
@@ -7152,7 +7137,7 @@
         <v>298</v>
       </c>
       <c r="JF8" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG8">
         <v>86400</v>
@@ -7172,10 +7157,10 @@
         <v>275</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -7184,7 +7169,7 @@
         <v>2.6</v>
       </c>
       <c r="J9">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -7196,7 +7181,7 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>3564000</v>
+        <v>5527000</v>
       </c>
       <c r="O9" t="s">
         <v>283</v>
@@ -7325,7 +7310,7 @@
         <v>1</v>
       </c>
       <c r="BG9">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH9" t="s">
         <v>296</v>
@@ -7451,7 +7436,7 @@
         <v>1</v>
       </c>
       <c r="CZ9">
-        <v>5600</v>
+        <v>8100</v>
       </c>
       <c r="DA9" t="s">
         <v>300</v>
@@ -7655,7 +7640,7 @@
         <v>1</v>
       </c>
       <c r="FV9">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW9" t="s">
         <v>304</v>
@@ -7718,13 +7703,40 @@
         <v>303</v>
       </c>
       <c r="GQ9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="GR9">
+        <v>1</v>
+      </c>
+      <c r="GS9" t="s">
+        <v>310</v>
+      </c>
+      <c r="GT9">
+        <v>75000</v>
+      </c>
+      <c r="GU9">
+        <v>7200</v>
+      </c>
+      <c r="GV9">
+        <v>11000</v>
+      </c>
+      <c r="GW9">
+        <v>100000</v>
+      </c>
+      <c r="GX9">
+        <v>0.9</v>
+      </c>
+      <c r="GY9">
+        <v>0.8</v>
+      </c>
+      <c r="GZ9" t="b">
+        <v>0</v>
+      </c>
+      <c r="HA9" t="b">
         <v>0</v>
       </c>
       <c r="HK9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL9">
         <v>0.05</v>
@@ -7739,18 +7751,36 @@
         <v>8.5</v>
       </c>
       <c r="HP9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR9" t="s">
         <v>303</v>
       </c>
       <c r="HS9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="HT9">
+        <v>1</v>
+      </c>
+      <c r="HU9">
+        <v>5500</v>
+      </c>
+      <c r="HV9">
+        <v>5500</v>
+      </c>
+      <c r="HW9">
+        <v>0.95</v>
+      </c>
+      <c r="HX9">
+        <v>0.1</v>
+      </c>
+      <c r="HY9" t="b">
+        <v>0</v>
+      </c>
+      <c r="HZ9" t="b">
         <v>0</v>
       </c>
       <c r="IA9" t="s">
@@ -7763,10 +7793,10 @@
         <v>1</v>
       </c>
       <c r="ID9">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE9">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF9">
         <v>0.95</v>
@@ -7778,43 +7808,43 @@
         <v>303</v>
       </c>
       <c r="II9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK9">
         <v>120</v>
       </c>
       <c r="IL9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM9">
         <v>120</v>
       </c>
       <c r="IN9" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO9">
         <v>86400</v>
       </c>
       <c r="IP9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ9">
         <v>120</v>
       </c>
       <c r="IR9" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS9">
         <v>120</v>
       </c>
       <c r="IT9" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU9">
-        <v>86400</v>
+        <v>57600</v>
       </c>
       <c r="IV9">
         <v>1</v>
@@ -7835,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="JB9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC9" t="s">
         <v>298</v>
@@ -7847,7 +7877,7 @@
         <v>298</v>
       </c>
       <c r="JF9" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG9">
         <v>86400</v>
@@ -7891,10 +7921,10 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <v>3125000</v>
+        <v>4402000</v>
       </c>
       <c r="O10" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="P10" t="s">
         <v>285</v>
@@ -8023,10 +8053,10 @@
         <v>19500000</v>
       </c>
       <c r="BH10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="BI10">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="BJ10" t="s">
         <v>298</v>
@@ -8146,16 +8176,16 @@
         <v>1</v>
       </c>
       <c r="CZ10">
-        <v>4900</v>
+        <v>7400</v>
       </c>
       <c r="DA10" t="s">
         <v>300</v>
       </c>
       <c r="DB10">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="DC10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="DD10" t="b">
         <v>0</v>
@@ -8353,7 +8383,7 @@
         <v>9800</v>
       </c>
       <c r="FW10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="FX10" t="s">
         <v>298</v>
@@ -8419,7 +8449,7 @@
         <v>0</v>
       </c>
       <c r="HK10" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL10">
         <v>0.05</v>
@@ -8434,10 +8464,10 @@
         <v>8.5</v>
       </c>
       <c r="HP10" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR10" t="s">
         <v>303</v>
@@ -8449,10 +8479,10 @@
         <v>1</v>
       </c>
       <c r="HU10">
-        <v>3100</v>
+        <v>4400</v>
       </c>
       <c r="HV10">
-        <v>3100</v>
+        <v>4400</v>
       </c>
       <c r="HW10">
         <v>0.95</v>
@@ -8491,40 +8521,40 @@
         <v>303</v>
       </c>
       <c r="II10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK10">
         <v>120</v>
       </c>
       <c r="IL10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM10">
         <v>120</v>
       </c>
       <c r="IN10" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO10">
         <v>86400</v>
       </c>
       <c r="IP10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ10">
         <v>120</v>
       </c>
       <c r="IR10" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS10">
         <v>120</v>
       </c>
       <c r="IT10" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU10">
         <v>86400</v>
@@ -8548,7 +8578,7 @@
         <v>1</v>
       </c>
       <c r="JB10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC10" t="s">
         <v>298</v>
@@ -8560,7 +8590,7 @@
         <v>298</v>
       </c>
       <c r="JF10" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG10">
         <v>86400</v>
@@ -8580,10 +8610,10 @@
         <v>277</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="H11">
         <v>2</v>
@@ -8592,7 +8622,7 @@
         <v>2.6</v>
       </c>
       <c r="J11">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -8604,10 +8634,10 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>5527000</v>
+        <v>3863000</v>
       </c>
       <c r="O11" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="P11" t="s">
         <v>285</v>
@@ -8733,10 +8763,10 @@
         <v>1</v>
       </c>
       <c r="BG11">
-        <v>19500000</v>
+        <v>5500000</v>
       </c>
       <c r="BH11" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="BI11">
         <v>55</v>
@@ -8859,7 +8889,7 @@
         <v>1</v>
       </c>
       <c r="CZ11">
-        <v>7200</v>
+        <v>5600</v>
       </c>
       <c r="DA11" t="s">
         <v>300</v>
@@ -9063,10 +9093,10 @@
         <v>1</v>
       </c>
       <c r="FV11">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="FW11" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="FX11" t="s">
         <v>298</v>
@@ -9126,67 +9156,13 @@
         <v>303</v>
       </c>
       <c r="GQ11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="GR11">
-        <v>2</v>
-      </c>
-      <c r="GS11" t="s">
-        <v>310</v>
-      </c>
-      <c r="GT11">
-        <v>50000</v>
-      </c>
-      <c r="GU11">
-        <v>7200</v>
-      </c>
-      <c r="GV11">
-        <v>7200</v>
-      </c>
-      <c r="GW11">
-        <v>50000</v>
-      </c>
-      <c r="GX11">
-        <v>0.9</v>
-      </c>
-      <c r="GY11">
-        <v>0.8</v>
-      </c>
-      <c r="GZ11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HA11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HB11" t="s">
-        <v>308</v>
-      </c>
-      <c r="HC11">
-        <v>75000</v>
-      </c>
-      <c r="HD11">
-        <v>7200</v>
-      </c>
-      <c r="HE11">
-        <v>11000</v>
-      </c>
-      <c r="HF11">
-        <v>100000</v>
-      </c>
-      <c r="HG11">
-        <v>0.9</v>
-      </c>
-      <c r="HH11">
-        <v>0.8</v>
-      </c>
-      <c r="HI11" t="b">
-        <v>0</v>
-      </c>
-      <c r="HJ11" t="b">
         <v>0</v>
       </c>
       <c r="HK11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="HL11">
         <v>0.05</v>
@@ -9201,10 +9177,10 @@
         <v>8.5</v>
       </c>
       <c r="HP11" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="HQ11" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="HR11" t="s">
         <v>303</v>
@@ -9216,10 +9192,10 @@
         <v>1</v>
       </c>
       <c r="HU11">
-        <v>5500</v>
+        <v>3900</v>
       </c>
       <c r="HV11">
-        <v>5500</v>
+        <v>3900</v>
       </c>
       <c r="HW11">
         <v>0.95</v>
@@ -9243,10 +9219,10 @@
         <v>1</v>
       </c>
       <c r="ID11">
-        <v>9800</v>
+        <v>2800</v>
       </c>
       <c r="IE11">
-        <v>19500</v>
+        <v>5500</v>
       </c>
       <c r="IF11">
         <v>0.95</v>
@@ -9258,43 +9234,43 @@
         <v>303</v>
       </c>
       <c r="II11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IJ11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IK11">
         <v>120</v>
       </c>
       <c r="IL11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IM11">
         <v>120</v>
       </c>
       <c r="IN11" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="IO11">
         <v>86400</v>
       </c>
       <c r="IP11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IQ11">
         <v>120</v>
       </c>
       <c r="IR11" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="IS11">
         <v>120</v>
       </c>
       <c r="IT11" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="IU11">
-        <v>57600</v>
+        <v>72000</v>
       </c>
       <c r="IV11">
         <v>1</v>
@@ -9315,7 +9291,7 @@
         <v>1</v>
       </c>
       <c r="JB11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JC11" t="s">
         <v>298</v>
@@ -9327,7 +9303,7 @@
         <v>298</v>
       </c>
       <c r="JF11" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="JG11">
         <v>86400</v>

</xml_diff>